<commit_message>
Added a route for Items
</commit_message>
<xml_diff>
--- a/infostorm_data.xlsx
+++ b/infostorm_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subham_bal\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanagaraj_m\Desktop\ThreeMuskeeteers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="B4:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>